<commit_message>
misc doc - updates because of changed functionality
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C33883
</commit_message>
<xml_diff>
--- a/Requirements/Misc/ecl_test_job_steps.xlsx
+++ b/Requirements/Misc/ecl_test_job_steps.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\eCoaching_V2\Requirements\Misc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Job Name</t>
   </si>
@@ -317,6 +322,68 @@
   </si>
   <si>
     <t>\\vrivscors01\BCC Scorecards\Coaching\WH\&lt;SiteLocation&gt;Warnings.csv</t>
+  </si>
+  <si>
+    <t>CoachingInactivations</t>
+  </si>
+  <si>
+    <t>Inactivations</t>
+  </si>
+  <si>
+    <t>Inactivations logs</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log.StatusID = 2 or
+EC.Warning_Log.StatusID = 2
+email notification sent to john;
+log file generated to \\vrivscors01\BCC Scorecards\Coaching\Inactivations\Processed</t>
+  </si>
+  <si>
+    <t>\\vrivscors01\BCC Scorecards\Coaching\Inactivations\eCL_Coaching_&lt;MMDDCCYY&gt;.csv
+\\vrivscors01\BCC Scorecards\Coaching\Inactivations\eCL_Warning_&lt;MMDDCCYY&gt;.csv</t>
+  </si>
+  <si>
+    <t>CoachingReminders</t>
+  </si>
+  <si>
+    <t>Reminders</t>
+  </si>
+  <si>
+    <t>Sends email reminders when certain logs have not been coached</t>
+  </si>
+  <si>
+    <t>selection determined by log source/reason/sub-reason/value</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log</t>
+  </si>
+  <si>
+    <t>CoachingSurveyGenerate</t>
+  </si>
+  <si>
+    <t>CoachingSurveyNotifications</t>
+  </si>
+  <si>
+    <t>SurveyGenerate</t>
+  </si>
+  <si>
+    <t>SurveyNotifications</t>
+  </si>
+  <si>
+    <t>Sends email notification regarding survey</t>
+  </si>
+  <si>
+    <t>Provides for selecting those logs which will be included in survey</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log.SurveySent = 0</t>
+  </si>
+  <si>
+    <t>EC.Coaching_Log.SurveySent = 1
+email notification sent to recipient</t>
+  </si>
+  <si>
+    <t>EC.Survey_Response_Detail</t>
   </si>
 </sst>
 </file>
@@ -422,6 +489,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -469,7 +539,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,7 +574,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -713,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -791,92 +861,188 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tfs3179 - ecl kudos feed and tfs3186 - ecl high 5 csat data feed
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C34726
</commit_message>
<xml_diff>
--- a/Requirements/Misc/ecl_test_job_steps.xlsx
+++ b/Requirements/Misc/ecl_test_job_steps.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="131">
   <si>
     <t>Job Name</t>
   </si>
@@ -384,6 +384,81 @@
   </si>
   <si>
     <t>EC.Survey_Response_Detail</t>
+  </si>
+  <si>
+    <t>CoachingGenericLoad</t>
+  </si>
+  <si>
+    <t>Generic file Load</t>
+  </si>
+  <si>
+    <t>Inports generic coaching logs</t>
+  </si>
+  <si>
+    <t>CoachingQualityOtherLoad</t>
+  </si>
+  <si>
+    <t>Quality Other Load</t>
+  </si>
+  <si>
+    <t>CoachingSurveyReminders</t>
+  </si>
+  <si>
+    <t>SurveyReminders</t>
+  </si>
+  <si>
+    <t>Sends reminder email notification regarding survey</t>
+  </si>
+  <si>
+    <t>CoachingTraining</t>
+  </si>
+  <si>
+    <t>Load Training Files</t>
+  </si>
+  <si>
+    <t>Imports quality reports information to create coaching logs</t>
+  </si>
+  <si>
+    <t>Imports training reports information to create coaching logs</t>
+  </si>
+  <si>
+    <t>\\vrivscors01\BCC Scorecards\Coaching\Generic\eCL_Generic_Feed_XXX&lt;YYYYMMDD&gt;.csv</t>
+  </si>
+  <si>
+    <t>\\vrivscors01\BCC Scorecards\Coaching\Quality\eCL_Quality_Feed_XXX&lt;YYYYMMDD&gt;.csv</t>
+  </si>
+  <si>
+    <t>\\vrivscors01\BCC Scorecards\Coaching\Training\eCL_Training_Feed_XXX&lt;YYYYMMDD&gt;.csv</t>
+  </si>
+  <si>
+    <t>EC.Generic_Coaching_Stage
+    EC.Generic_Coaching_Rejected
+    EC.Generic_Coaching_Fact
+        EC.Coaching_Log
+        EC.Coaching_Log_Reason</t>
+  </si>
+  <si>
+    <t>EC.Quality_Other_Coaching_Stage
+    EC.Quality_Other_Coacing_Rejected
+    EC.Quality_Other_Coaching_Fact
+        EC.Coaching_Log
+        EC.Coaching_Log_Reason</t>
+  </si>
+  <si>
+    <t>EC.Training_Coaching_Stage
+    EC.Training_Coacing_Rejected
+    EC.Training_Coaching_Fact
+        EC.Coaching_Log
+        EC.Coaching_Log_Reason</t>
+  </si>
+  <si>
+    <t>EC.Survey_Response_Header.ReminderSent = 1
+EC.Survey_Response_Header.ReminderDate = email date
+EC.Survey_Response_Header.ReminderCount = +1
+email reminder notification sent to recipient</t>
+  </si>
+  <si>
+    <t>EC.Survey_Response_Header.NotificationDate = today's date - 3</t>
   </si>
 </sst>
 </file>
@@ -783,7 +858,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -861,21 +936,21 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -885,69 +960,69 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>80</v>
+        <v>73</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,21 +1032,21 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -981,21 +1056,21 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,44 +1082,147 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>